<commit_message>
Running pipeline, but needs more fixes to small data mismatches between datasets
</commit_message>
<xml_diff>
--- a/src/bunnyhop/data/DLA_CityNames.xlsx
+++ b/src/bunnyhop/data/DLA_CityNames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateca-my.sharepoint.com/personal/nick_santos_state_ca_gov/Documents/Documents/Code/BunnyHop/tests/data/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateca-my.sharepoint.com/personal/nick_santos_state_ca_gov/Documents/Code/BunnyHop/src/bunnyhop/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_E8F227924047C42EE0646437535DCE3AE7CD5C31" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85D082F1-21E2-488B-9E63-2FF19A418481}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_E8F227924047C42EE0646437535DCE3AE7CD5C31" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3F25746-77C5-406A-9A55-82A2FC80AA1F}"/>
   <bookViews>
-    <workbookView xWindow="35115" yWindow="12300" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CityNames" sheetId="1" r:id="rId1"/>
@@ -6287,11 +6287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J483"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I498" sqref="I498"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6340,7 +6339,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>59</v>
       </c>
@@ -6372,7 +6371,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>60</v>
       </c>
@@ -6404,7 +6403,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>61</v>
       </c>
@@ -6436,7 +6435,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>62</v>
       </c>
@@ -6468,7 +6467,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>63</v>
       </c>
@@ -6500,7 +6499,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>64</v>
       </c>
@@ -6532,7 +6531,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>65</v>
       </c>
@@ -6564,7 +6563,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>66</v>
       </c>
@@ -6596,7 +6595,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>67</v>
       </c>
@@ -6628,7 +6627,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>68</v>
       </c>
@@ -6660,7 +6659,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>69</v>
       </c>
@@ -6692,7 +6691,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>70</v>
       </c>
@@ -6724,7 +6723,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>71</v>
       </c>
@@ -6756,7 +6755,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>72</v>
       </c>
@@ -6788,7 +6787,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>73</v>
       </c>
@@ -6820,7 +6819,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>74</v>
       </c>
@@ -6852,7 +6851,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>75</v>
       </c>
@@ -6884,7 +6883,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>76</v>
       </c>
@@ -6916,7 +6915,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>77</v>
       </c>
@@ -6948,7 +6947,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>78</v>
       </c>
@@ -6980,7 +6979,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>79</v>
       </c>
@@ -7012,7 +7011,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>80</v>
       </c>
@@ -7044,7 +7043,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>81</v>
       </c>
@@ -7076,7 +7075,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>82</v>
       </c>
@@ -7108,7 +7107,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>83</v>
       </c>
@@ -7140,7 +7139,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>84</v>
       </c>
@@ -7172,7 +7171,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>85</v>
       </c>
@@ -7204,7 +7203,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>86</v>
       </c>
@@ -7236,7 +7235,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>87</v>
       </c>
@@ -7268,7 +7267,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>88</v>
       </c>
@@ -7300,7 +7299,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>89</v>
       </c>
@@ -7332,7 +7331,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>90</v>
       </c>
@@ -7364,7 +7363,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>91</v>
       </c>
@@ -7396,7 +7395,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>92</v>
       </c>
@@ -7428,7 +7427,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>93</v>
       </c>
@@ -7460,7 +7459,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>94</v>
       </c>
@@ -7492,7 +7491,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>95</v>
       </c>
@@ -7524,7 +7523,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>96</v>
       </c>
@@ -7556,7 +7555,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>97</v>
       </c>
@@ -7588,7 +7587,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>98</v>
       </c>
@@ -7620,7 +7619,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>99</v>
       </c>
@@ -7652,7 +7651,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>100</v>
       </c>
@@ -7684,7 +7683,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>101</v>
       </c>
@@ -7716,7 +7715,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>102</v>
       </c>
@@ -7748,7 +7747,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>103</v>
       </c>
@@ -7780,7 +7779,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>104</v>
       </c>
@@ -7812,7 +7811,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>105</v>
       </c>
@@ -7844,7 +7843,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>106</v>
       </c>
@@ -7876,7 +7875,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>107</v>
       </c>
@@ -7908,7 +7907,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>108</v>
       </c>
@@ -7940,7 +7939,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>109</v>
       </c>
@@ -7972,7 +7971,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>110</v>
       </c>
@@ -8004,7 +8003,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>111</v>
       </c>
@@ -8036,7 +8035,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>112</v>
       </c>
@@ -8068,7 +8067,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>113</v>
       </c>
@@ -8100,7 +8099,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>114</v>
       </c>
@@ -8132,7 +8131,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>115</v>
       </c>
@@ -8164,7 +8163,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>116</v>
       </c>
@@ -8196,7 +8195,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>117</v>
       </c>
@@ -8228,7 +8227,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>118</v>
       </c>
@@ -8260,7 +8259,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>119</v>
       </c>
@@ -8292,7 +8291,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>120</v>
       </c>
@@ -8324,7 +8323,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>121</v>
       </c>
@@ -8356,7 +8355,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>122</v>
       </c>
@@ -8388,7 +8387,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>123</v>
       </c>
@@ -8420,7 +8419,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>124</v>
       </c>
@@ -8452,7 +8451,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>125</v>
       </c>
@@ -8484,7 +8483,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>126</v>
       </c>
@@ -8516,7 +8515,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>127</v>
       </c>
@@ -8548,7 +8547,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>128</v>
       </c>
@@ -8580,7 +8579,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>129</v>
       </c>
@@ -8612,7 +8611,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>130</v>
       </c>
@@ -8644,7 +8643,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>131</v>
       </c>
@@ -8676,7 +8675,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>132</v>
       </c>
@@ -8708,7 +8707,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>133</v>
       </c>
@@ -8740,7 +8739,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>134</v>
       </c>
@@ -8772,7 +8771,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>135</v>
       </c>
@@ -8804,7 +8803,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>136</v>
       </c>
@@ -8836,7 +8835,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>137</v>
       </c>
@@ -8868,7 +8867,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>138</v>
       </c>
@@ -8900,7 +8899,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>139</v>
       </c>
@@ -8932,7 +8931,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>140</v>
       </c>
@@ -8964,7 +8963,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>141</v>
       </c>
@@ -8996,7 +8995,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>142</v>
       </c>
@@ -9028,7 +9027,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>143</v>
       </c>
@@ -9060,7 +9059,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>144</v>
       </c>
@@ -9092,7 +9091,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>145</v>
       </c>
@@ -9124,7 +9123,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>146</v>
       </c>
@@ -9156,7 +9155,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>147</v>
       </c>
@@ -9188,7 +9187,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>148</v>
       </c>
@@ -9220,7 +9219,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>149</v>
       </c>
@@ -9252,7 +9251,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>150</v>
       </c>
@@ -9284,7 +9283,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>151</v>
       </c>
@@ -9316,7 +9315,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>152</v>
       </c>
@@ -9348,7 +9347,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>153</v>
       </c>
@@ -9380,7 +9379,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>154</v>
       </c>
@@ -9412,7 +9411,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>155</v>
       </c>
@@ -9444,7 +9443,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>156</v>
       </c>
@@ -9476,7 +9475,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>157</v>
       </c>
@@ -9508,7 +9507,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>158</v>
       </c>
@@ -9540,7 +9539,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>159</v>
       </c>
@@ -9572,7 +9571,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>160</v>
       </c>
@@ -9604,7 +9603,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>161</v>
       </c>
@@ -9636,7 +9635,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>162</v>
       </c>
@@ -9668,7 +9667,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>163</v>
       </c>
@@ -9700,7 +9699,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>164</v>
       </c>
@@ -9732,7 +9731,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>165</v>
       </c>
@@ -9764,7 +9763,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>166</v>
       </c>
@@ -9796,7 +9795,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>167</v>
       </c>
@@ -9828,7 +9827,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>168</v>
       </c>
@@ -9860,7 +9859,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>169</v>
       </c>
@@ -9892,7 +9891,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>170</v>
       </c>
@@ -9924,7 +9923,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>171</v>
       </c>
@@ -9956,7 +9955,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>172</v>
       </c>
@@ -9988,7 +9987,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>173</v>
       </c>
@@ -10020,7 +10019,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>174</v>
       </c>
@@ -10052,7 +10051,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>175</v>
       </c>
@@ -10084,7 +10083,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>176</v>
       </c>
@@ -10116,7 +10115,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>177</v>
       </c>
@@ -10148,7 +10147,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>178</v>
       </c>
@@ -10180,7 +10179,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>179</v>
       </c>
@@ -10212,7 +10211,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>180</v>
       </c>
@@ -10244,7 +10243,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>181</v>
       </c>
@@ -10276,7 +10275,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>182</v>
       </c>
@@ -10308,7 +10307,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>183</v>
       </c>
@@ -10340,7 +10339,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>184</v>
       </c>
@@ -10372,7 +10371,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>185</v>
       </c>
@@ -10404,7 +10403,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>186</v>
       </c>
@@ -10436,7 +10435,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>187</v>
       </c>
@@ -10468,7 +10467,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>188</v>
       </c>
@@ -10500,7 +10499,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>189</v>
       </c>
@@ -10532,7 +10531,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>190</v>
       </c>
@@ -10564,7 +10563,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>191</v>
       </c>
@@ -10596,7 +10595,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>192</v>
       </c>
@@ -10628,7 +10627,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>193</v>
       </c>
@@ -10660,7 +10659,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>194</v>
       </c>
@@ -10692,7 +10691,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>195</v>
       </c>
@@ -10724,7 +10723,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>196</v>
       </c>
@@ -10756,7 +10755,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>197</v>
       </c>
@@ -10788,7 +10787,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>198</v>
       </c>
@@ -10820,7 +10819,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>199</v>
       </c>
@@ -10852,7 +10851,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>200</v>
       </c>
@@ -10884,7 +10883,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>201</v>
       </c>
@@ -10916,7 +10915,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>202</v>
       </c>
@@ -10948,7 +10947,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>203</v>
       </c>
@@ -10980,7 +10979,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>204</v>
       </c>
@@ -11012,7 +11011,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>205</v>
       </c>
@@ -11044,7 +11043,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>206</v>
       </c>
@@ -11076,7 +11075,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>207</v>
       </c>
@@ -11108,7 +11107,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>208</v>
       </c>
@@ -11140,7 +11139,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>209</v>
       </c>
@@ -11172,7 +11171,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>210</v>
       </c>
@@ -11204,7 +11203,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>211</v>
       </c>
@@ -11236,7 +11235,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>212</v>
       </c>
@@ -11268,7 +11267,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>213</v>
       </c>
@@ -11300,7 +11299,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>214</v>
       </c>
@@ -11332,7 +11331,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>215</v>
       </c>
@@ -11364,7 +11363,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>216</v>
       </c>
@@ -11396,7 +11395,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>217</v>
       </c>
@@ -11428,7 +11427,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>218</v>
       </c>
@@ -11460,7 +11459,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>219</v>
       </c>
@@ -11492,7 +11491,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>220</v>
       </c>
@@ -11524,7 +11523,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>221</v>
       </c>
@@ -11556,7 +11555,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>222</v>
       </c>
@@ -11588,7 +11587,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>223</v>
       </c>
@@ -11620,7 +11619,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>224</v>
       </c>
@@ -11652,7 +11651,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>225</v>
       </c>
@@ -11684,7 +11683,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>226</v>
       </c>
@@ -11716,7 +11715,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>227</v>
       </c>
@@ -11748,7 +11747,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>228</v>
       </c>
@@ -11780,7 +11779,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>229</v>
       </c>
@@ -11812,7 +11811,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>230</v>
       </c>
@@ -11844,7 +11843,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>231</v>
       </c>
@@ -11876,7 +11875,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>232</v>
       </c>
@@ -11908,7 +11907,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>233</v>
       </c>
@@ -11940,7 +11939,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>234</v>
       </c>
@@ -11972,7 +11971,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>235</v>
       </c>
@@ -12004,7 +12003,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>236</v>
       </c>
@@ -12036,7 +12035,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>237</v>
       </c>
@@ -12068,7 +12067,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>238</v>
       </c>
@@ -12100,7 +12099,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>239</v>
       </c>
@@ -12132,7 +12131,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>240</v>
       </c>
@@ -12164,7 +12163,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>241</v>
       </c>
@@ -12196,7 +12195,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>242</v>
       </c>
@@ -12228,7 +12227,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>243</v>
       </c>
@@ -12260,7 +12259,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>244</v>
       </c>
@@ -12292,7 +12291,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>245</v>
       </c>
@@ -12324,7 +12323,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>246</v>
       </c>
@@ -12356,7 +12355,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>247</v>
       </c>
@@ -12388,7 +12387,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>248</v>
       </c>
@@ -12420,7 +12419,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>249</v>
       </c>
@@ -12452,7 +12451,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>250</v>
       </c>
@@ -12484,7 +12483,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>251</v>
       </c>
@@ -12516,7 +12515,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>252</v>
       </c>
@@ -12548,7 +12547,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>253</v>
       </c>
@@ -12580,7 +12579,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>254</v>
       </c>
@@ -12612,7 +12611,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>255</v>
       </c>
@@ -12644,7 +12643,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>256</v>
       </c>
@@ -12676,7 +12675,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>257</v>
       </c>
@@ -12708,7 +12707,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>258</v>
       </c>
@@ -12740,7 +12739,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>259</v>
       </c>
@@ -12772,7 +12771,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>260</v>
       </c>
@@ -12804,7 +12803,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>261</v>
       </c>
@@ -12836,7 +12835,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>262</v>
       </c>
@@ -12868,7 +12867,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>263</v>
       </c>
@@ -12900,7 +12899,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>264</v>
       </c>
@@ -12932,7 +12931,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>265</v>
       </c>
@@ -12964,7 +12963,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>266</v>
       </c>
@@ -12996,7 +12995,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>267</v>
       </c>
@@ -13028,7 +13027,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>268</v>
       </c>
@@ -13060,7 +13059,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>269</v>
       </c>
@@ -13092,7 +13091,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>270</v>
       </c>
@@ -13124,7 +13123,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>271</v>
       </c>
@@ -13156,7 +13155,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>272</v>
       </c>
@@ -13188,7 +13187,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>273</v>
       </c>
@@ -13220,7 +13219,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>274</v>
       </c>
@@ -13252,7 +13251,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>275</v>
       </c>
@@ -13284,7 +13283,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>276</v>
       </c>
@@ -13316,7 +13315,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>277</v>
       </c>
@@ -13348,7 +13347,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>278</v>
       </c>
@@ -13380,7 +13379,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>279</v>
       </c>
@@ -13412,7 +13411,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>280</v>
       </c>
@@ -13444,7 +13443,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>281</v>
       </c>
@@ -13476,7 +13475,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>282</v>
       </c>
@@ -13508,7 +13507,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>283</v>
       </c>
@@ -13540,7 +13539,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>284</v>
       </c>
@@ -13572,7 +13571,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>285</v>
       </c>
@@ -13604,7 +13603,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>286</v>
       </c>
@@ -13636,7 +13635,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>287</v>
       </c>
@@ -13668,7 +13667,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>288</v>
       </c>
@@ -13700,7 +13699,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>289</v>
       </c>
@@ -13732,7 +13731,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>290</v>
       </c>
@@ -13764,7 +13763,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>291</v>
       </c>
@@ -13796,7 +13795,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>292</v>
       </c>
@@ -13828,7 +13827,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>293</v>
       </c>
@@ -13860,7 +13859,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>294</v>
       </c>
@@ -13892,7 +13891,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>295</v>
       </c>
@@ -13924,7 +13923,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>296</v>
       </c>
@@ -13956,7 +13955,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>297</v>
       </c>
@@ -13988,7 +13987,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>298</v>
       </c>
@@ -14020,7 +14019,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>299</v>
       </c>
@@ -14052,7 +14051,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>300</v>
       </c>
@@ -14084,7 +14083,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>301</v>
       </c>
@@ -14116,7 +14115,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>302</v>
       </c>
@@ -14148,7 +14147,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>303</v>
       </c>
@@ -14180,7 +14179,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>304</v>
       </c>
@@ -14212,7 +14211,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>305</v>
       </c>
@@ -14244,7 +14243,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>306</v>
       </c>
@@ -14276,7 +14275,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="250" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>307</v>
       </c>
@@ -14308,7 +14307,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>308</v>
       </c>
@@ -14340,7 +14339,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>309</v>
       </c>
@@ -14372,7 +14371,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>310</v>
       </c>
@@ -14404,7 +14403,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>311</v>
       </c>
@@ -14436,7 +14435,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>312</v>
       </c>
@@ -14468,7 +14467,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>313</v>
       </c>
@@ -14500,7 +14499,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>314</v>
       </c>
@@ -14532,7 +14531,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="258" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>315</v>
       </c>
@@ -14564,7 +14563,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="259" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>316</v>
       </c>
@@ -14596,7 +14595,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="260" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>317</v>
       </c>
@@ -14628,7 +14627,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="261" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>318</v>
       </c>
@@ -14660,7 +14659,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="262" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>319</v>
       </c>
@@ -14692,7 +14691,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="263" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>320</v>
       </c>
@@ -14724,7 +14723,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="264" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>321</v>
       </c>
@@ -14756,7 +14755,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="265" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>322</v>
       </c>
@@ -14788,7 +14787,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="266" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>323</v>
       </c>
@@ -14820,7 +14819,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="267" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>324</v>
       </c>
@@ -14852,7 +14851,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="268" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>325</v>
       </c>
@@ -14884,7 +14883,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="269" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>326</v>
       </c>
@@ -14916,7 +14915,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="270" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>327</v>
       </c>
@@ -14948,7 +14947,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="271" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>328</v>
       </c>
@@ -14980,7 +14979,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="272" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>329</v>
       </c>
@@ -15012,7 +15011,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="273" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>330</v>
       </c>
@@ -15044,7 +15043,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="274" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>331</v>
       </c>
@@ -15076,7 +15075,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="275" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>332</v>
       </c>
@@ -15108,7 +15107,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="276" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>333</v>
       </c>
@@ -15140,7 +15139,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="277" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>334</v>
       </c>
@@ -15172,7 +15171,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="278" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>335</v>
       </c>
@@ -15204,7 +15203,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="279" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>336</v>
       </c>
@@ -15236,7 +15235,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="280" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>337</v>
       </c>
@@ -15268,7 +15267,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="281" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>338</v>
       </c>
@@ -15300,7 +15299,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="282" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>339</v>
       </c>
@@ -15332,7 +15331,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="283" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>340</v>
       </c>
@@ -15364,7 +15363,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="284" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>341</v>
       </c>
@@ -15396,7 +15395,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="285" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>342</v>
       </c>
@@ -15428,7 +15427,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="286" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>343</v>
       </c>
@@ -15460,7 +15459,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="287" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>344</v>
       </c>
@@ -15492,7 +15491,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="288" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>345</v>
       </c>
@@ -15524,7 +15523,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="289" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>346</v>
       </c>
@@ -15556,7 +15555,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="290" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>347</v>
       </c>
@@ -15588,7 +15587,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="291" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>348</v>
       </c>
@@ -15620,7 +15619,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="292" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>349</v>
       </c>
@@ -15652,7 +15651,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="293" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>350</v>
       </c>
@@ -15684,7 +15683,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="294" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>351</v>
       </c>
@@ -15716,7 +15715,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="295" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>352</v>
       </c>
@@ -15748,7 +15747,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="296" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>353</v>
       </c>
@@ -15780,7 +15779,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="297" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>354</v>
       </c>
@@ -15812,7 +15811,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="298" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>355</v>
       </c>
@@ -15844,7 +15843,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="299" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>356</v>
       </c>
@@ -15876,7 +15875,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="300" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>357</v>
       </c>
@@ -15908,7 +15907,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="301" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>358</v>
       </c>
@@ -15940,7 +15939,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="302" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>359</v>
       </c>
@@ -15972,7 +15971,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="303" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>360</v>
       </c>
@@ -16004,7 +16003,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="304" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>361</v>
       </c>
@@ -16036,7 +16035,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="305" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>362</v>
       </c>
@@ -16068,7 +16067,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="306" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>363</v>
       </c>
@@ -16100,7 +16099,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="307" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>364</v>
       </c>
@@ -16132,7 +16131,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="308" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>365</v>
       </c>
@@ -16164,7 +16163,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="309" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>366</v>
       </c>
@@ -16196,7 +16195,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="310" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>367</v>
       </c>
@@ -16228,7 +16227,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="311" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>368</v>
       </c>
@@ -16260,7 +16259,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="312" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>369</v>
       </c>
@@ -16292,7 +16291,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="313" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>370</v>
       </c>
@@ -16324,7 +16323,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="314" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>371</v>
       </c>
@@ -16356,7 +16355,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="315" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>372</v>
       </c>
@@ -16388,7 +16387,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="316" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>373</v>
       </c>
@@ -16420,7 +16419,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="317" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>374</v>
       </c>
@@ -16452,7 +16451,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="318" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>375</v>
       </c>
@@ -16484,7 +16483,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="319" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>376</v>
       </c>
@@ -16516,7 +16515,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="320" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>377</v>
       </c>
@@ -16548,7 +16547,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="321" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>378</v>
       </c>
@@ -16580,7 +16579,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="322" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>379</v>
       </c>
@@ -16612,7 +16611,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="323" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>380</v>
       </c>
@@ -16644,7 +16643,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="324" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>381</v>
       </c>
@@ -16676,7 +16675,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="325" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>382</v>
       </c>
@@ -16708,7 +16707,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="326" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>383</v>
       </c>
@@ -16740,7 +16739,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="327" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>384</v>
       </c>
@@ -16772,7 +16771,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="328" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>385</v>
       </c>
@@ -16804,7 +16803,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="329" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>386</v>
       </c>
@@ -16836,7 +16835,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="330" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>387</v>
       </c>
@@ -16868,7 +16867,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="331" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>388</v>
       </c>
@@ -16900,7 +16899,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="332" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>389</v>
       </c>
@@ -16932,7 +16931,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="333" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>390</v>
       </c>
@@ -16964,7 +16963,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="334" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>391</v>
       </c>
@@ -16996,7 +16995,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="335" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>392</v>
       </c>
@@ -17028,7 +17027,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="336" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>393</v>
       </c>
@@ -17060,7 +17059,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="337" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>394</v>
       </c>
@@ -17092,7 +17091,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="338" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>395</v>
       </c>
@@ -17124,7 +17123,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="339" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>396</v>
       </c>
@@ -17156,7 +17155,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="340" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>397</v>
       </c>
@@ -17188,7 +17187,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="341" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>398</v>
       </c>
@@ -17220,7 +17219,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="342" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>399</v>
       </c>
@@ -17252,7 +17251,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="343" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>400</v>
       </c>
@@ -17284,7 +17283,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="344" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>401</v>
       </c>
@@ -17316,7 +17315,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="345" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>402</v>
       </c>
@@ -17348,7 +17347,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="346" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>403</v>
       </c>
@@ -17380,7 +17379,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="347" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>404</v>
       </c>
@@ -17412,7 +17411,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="348" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>405</v>
       </c>
@@ -17444,7 +17443,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="349" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>406</v>
       </c>
@@ -17476,7 +17475,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="350" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>407</v>
       </c>
@@ -17508,7 +17507,7 @@
         <v>1446</v>
       </c>
     </row>
-    <row r="351" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>408</v>
       </c>
@@ -17540,7 +17539,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="352" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>409</v>
       </c>
@@ -17572,7 +17571,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="353" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>410</v>
       </c>
@@ -17604,7 +17603,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="354" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>411</v>
       </c>
@@ -17636,7 +17635,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="355" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>412</v>
       </c>
@@ -17668,7 +17667,7 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="356" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>413</v>
       </c>
@@ -17700,7 +17699,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="357" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>414</v>
       </c>
@@ -17732,7 +17731,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="358" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>415</v>
       </c>
@@ -17764,7 +17763,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="359" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>416</v>
       </c>
@@ -17796,7 +17795,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="360" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>417</v>
       </c>
@@ -17828,7 +17827,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="361" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>418</v>
       </c>
@@ -17860,7 +17859,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="362" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>419</v>
       </c>
@@ -17892,7 +17891,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="363" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>420</v>
       </c>
@@ -17924,7 +17923,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="364" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>421</v>
       </c>
@@ -17956,7 +17955,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="365" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>422</v>
       </c>
@@ -17988,7 +17987,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="366" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>423</v>
       </c>
@@ -18020,7 +18019,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="367" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>424</v>
       </c>
@@ -18052,7 +18051,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="368" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>425</v>
       </c>
@@ -18084,7 +18083,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="369" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>426</v>
       </c>
@@ -18116,7 +18115,7 @@
         <v>1518</v>
       </c>
     </row>
-    <row r="370" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>427</v>
       </c>
@@ -18148,7 +18147,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="371" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>428</v>
       </c>
@@ -18180,7 +18179,7 @@
         <v>1526</v>
       </c>
     </row>
-    <row r="372" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>429</v>
       </c>
@@ -18212,7 +18211,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="373" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>430</v>
       </c>
@@ -18244,7 +18243,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="374" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>431</v>
       </c>
@@ -18276,7 +18275,7 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="375" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>432</v>
       </c>
@@ -18308,7 +18307,7 @@
         <v>1541</v>
       </c>
     </row>
-    <row r="376" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>433</v>
       </c>
@@ -18340,7 +18339,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="377" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>434</v>
       </c>
@@ -18372,7 +18371,7 @@
         <v>1549</v>
       </c>
     </row>
-    <row r="378" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>435</v>
       </c>
@@ -18404,7 +18403,7 @@
         <v>1553</v>
       </c>
     </row>
-    <row r="379" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>436</v>
       </c>
@@ -18436,7 +18435,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="380" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>437</v>
       </c>
@@ -18468,7 +18467,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="381" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>438</v>
       </c>
@@ -18500,7 +18499,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="382" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>439</v>
       </c>
@@ -18532,7 +18531,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="383" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>440</v>
       </c>
@@ -18564,7 +18563,7 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="384" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>441</v>
       </c>
@@ -18596,7 +18595,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="385" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>442</v>
       </c>
@@ -18628,7 +18627,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="386" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>443</v>
       </c>
@@ -18660,7 +18659,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="387" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>444</v>
       </c>
@@ -18692,7 +18691,7 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="388" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>445</v>
       </c>
@@ -18724,7 +18723,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="389" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>446</v>
       </c>
@@ -18756,7 +18755,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="390" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>447</v>
       </c>
@@ -18788,7 +18787,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="391" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>448</v>
       </c>
@@ -18820,7 +18819,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="392" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>449</v>
       </c>
@@ -18852,7 +18851,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="393" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>450</v>
       </c>
@@ -18884,7 +18883,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="394" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>451</v>
       </c>
@@ -18916,7 +18915,7 @@
         <v>1612</v>
       </c>
     </row>
-    <row r="395" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>452</v>
       </c>
@@ -18948,7 +18947,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="396" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>453</v>
       </c>
@@ -18980,7 +18979,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="397" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>454</v>
       </c>
@@ -19012,7 +19011,7 @@
         <v>1624</v>
       </c>
     </row>
-    <row r="398" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>455</v>
       </c>
@@ -19044,7 +19043,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="399" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>456</v>
       </c>
@@ -19076,7 +19075,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="400" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>457</v>
       </c>
@@ -19108,7 +19107,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="401" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>458</v>
       </c>
@@ -19140,7 +19139,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="402" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>459</v>
       </c>
@@ -19172,7 +19171,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="403" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>460</v>
       </c>
@@ -19204,7 +19203,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="404" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>461</v>
       </c>
@@ -19236,7 +19235,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="405" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>462</v>
       </c>
@@ -19268,7 +19267,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="406" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>463</v>
       </c>
@@ -19300,7 +19299,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="407" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>464</v>
       </c>
@@ -19332,7 +19331,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="408" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>465</v>
       </c>
@@ -19364,7 +19363,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="409" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>466</v>
       </c>
@@ -19396,7 +19395,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="410" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>467</v>
       </c>
@@ -19428,7 +19427,7 @@
         <v>1676</v>
       </c>
     </row>
-    <row r="411" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>468</v>
       </c>
@@ -19460,7 +19459,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="412" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>469</v>
       </c>
@@ -19492,7 +19491,7 @@
         <v>1683</v>
       </c>
     </row>
-    <row r="413" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>470</v>
       </c>
@@ -19524,7 +19523,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="414" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>471</v>
       </c>
@@ -19556,7 +19555,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="415" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>472</v>
       </c>
@@ -19588,7 +19587,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="416" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>473</v>
       </c>
@@ -19620,7 +19619,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="417" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>474</v>
       </c>
@@ -19652,7 +19651,7 @@
         <v>1703</v>
       </c>
     </row>
-    <row r="418" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>475</v>
       </c>
@@ -19684,7 +19683,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="419" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>476</v>
       </c>
@@ -19716,7 +19715,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="420" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>477</v>
       </c>
@@ -19748,7 +19747,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="421" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>478</v>
       </c>
@@ -19780,7 +19779,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="422" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>479</v>
       </c>
@@ -19812,7 +19811,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="423" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>480</v>
       </c>
@@ -19844,7 +19843,7 @@
         <v>1727</v>
       </c>
     </row>
-    <row r="424" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>481</v>
       </c>
@@ -19876,7 +19875,7 @@
         <v>1731</v>
       </c>
     </row>
-    <row r="425" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>482</v>
       </c>
@@ -19908,7 +19907,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="426" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>483</v>
       </c>
@@ -19940,7 +19939,7 @@
         <v>1740</v>
       </c>
     </row>
-    <row r="427" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>484</v>
       </c>
@@ -19972,7 +19971,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="428" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>485</v>
       </c>
@@ -20004,7 +20003,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="429" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>486</v>
       </c>
@@ -20036,7 +20035,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="430" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>487</v>
       </c>
@@ -20068,7 +20067,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="431" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>488</v>
       </c>
@@ -20100,7 +20099,7 @@
         <v>1759</v>
       </c>
     </row>
-    <row r="432" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>489</v>
       </c>
@@ -20132,7 +20131,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="433" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>490</v>
       </c>
@@ -20164,7 +20163,7 @@
         <v>1767</v>
       </c>
     </row>
-    <row r="434" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>491</v>
       </c>
@@ -20196,7 +20195,7 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="435" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>492</v>
       </c>
@@ -20228,7 +20227,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="436" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>493</v>
       </c>
@@ -20260,7 +20259,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="437" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>494</v>
       </c>
@@ -20292,7 +20291,7 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="438" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>495</v>
       </c>
@@ -20324,7 +20323,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="439" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>496</v>
       </c>
@@ -20356,7 +20355,7 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="440" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>497</v>
       </c>
@@ -20388,7 +20387,7 @@
         <v>1794</v>
       </c>
     </row>
-    <row r="441" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>498</v>
       </c>
@@ -20420,7 +20419,7 @@
         <v>1798</v>
       </c>
     </row>
-    <row r="442" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>499</v>
       </c>
@@ -20452,7 +20451,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="443" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>500</v>
       </c>
@@ -20484,7 +20483,7 @@
         <v>1806</v>
       </c>
     </row>
-    <row r="444" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>501</v>
       </c>
@@ -20516,7 +20515,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="445" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>502</v>
       </c>
@@ -20548,7 +20547,7 @@
         <v>1814</v>
       </c>
     </row>
-    <row r="446" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>503</v>
       </c>
@@ -20580,7 +20579,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="447" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>504</v>
       </c>
@@ -20612,7 +20611,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="448" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>505</v>
       </c>
@@ -20644,7 +20643,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="449" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>506</v>
       </c>
@@ -20676,7 +20675,7 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="450" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>507</v>
       </c>
@@ -20708,7 +20707,7 @@
         <v>1833</v>
       </c>
     </row>
-    <row r="451" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>508</v>
       </c>
@@ -20740,7 +20739,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="452" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>509</v>
       </c>
@@ -20804,7 +20803,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="454" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>511</v>
       </c>
@@ -20836,7 +20835,7 @@
         <v>1849</v>
       </c>
     </row>
-    <row r="455" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>512</v>
       </c>
@@ -20868,7 +20867,7 @@
         <v>1853</v>
       </c>
     </row>
-    <row r="456" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>513</v>
       </c>
@@ -20900,7 +20899,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="457" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>514</v>
       </c>
@@ -20932,7 +20931,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="458" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>515</v>
       </c>
@@ -20964,7 +20963,7 @@
         <v>1865</v>
       </c>
     </row>
-    <row r="459" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>516</v>
       </c>
@@ -20996,7 +20995,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="460" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>517</v>
       </c>
@@ -21028,7 +21027,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="461" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>518</v>
       </c>
@@ -21060,7 +21059,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="462" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>519</v>
       </c>
@@ -21092,7 +21091,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="463" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>520</v>
       </c>
@@ -21124,7 +21123,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="464" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>521</v>
       </c>
@@ -21156,7 +21155,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="465" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>522</v>
       </c>
@@ -21188,7 +21187,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="466" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>523</v>
       </c>
@@ -21220,7 +21219,7 @@
         <v>1897</v>
       </c>
     </row>
-    <row r="467" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>524</v>
       </c>
@@ -21252,7 +21251,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="468" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>525</v>
       </c>
@@ -21284,7 +21283,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="469" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>526</v>
       </c>
@@ -21316,7 +21315,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="470" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>527</v>
       </c>
@@ -21348,7 +21347,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="471" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>528</v>
       </c>
@@ -21380,7 +21379,7 @@
         <v>1917</v>
       </c>
     </row>
-    <row r="472" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>529</v>
       </c>
@@ -21412,7 +21411,7 @@
         <v>1921</v>
       </c>
     </row>
-    <row r="473" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>530</v>
       </c>
@@ -21444,7 +21443,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="474" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>531</v>
       </c>
@@ -21476,7 +21475,7 @@
         <v>1929</v>
       </c>
     </row>
-    <row r="475" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>532</v>
       </c>
@@ -21508,7 +21507,7 @@
         <v>1933</v>
       </c>
     </row>
-    <row r="476" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>533</v>
       </c>
@@ -21540,7 +21539,7 @@
         <v>1937</v>
       </c>
     </row>
-    <row r="477" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>534</v>
       </c>
@@ -21572,7 +21571,7 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="478" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>535</v>
       </c>
@@ -21604,7 +21603,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="479" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>536</v>
       </c>
@@ -21636,7 +21635,7 @@
         <v>1949</v>
       </c>
     </row>
-    <row r="480" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>537</v>
       </c>
@@ -21668,7 +21667,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="481" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>538</v>
       </c>
@@ -21700,7 +21699,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="482" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A482">
         <v>539</v>
       </c>
@@ -21732,7 +21731,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="483" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A483">
         <v>540</v>
       </c>
@@ -21765,13 +21764,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J483" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="0682954"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J483" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J483">
     <sortCondition ref="C7:C483"/>
   </sortState>

</xml_diff>